<commit_message>
Updated some rounding to meet AJPH requirements.
</commit_message>
<xml_diff>
--- a/Figures_Tables/tables.xlsx
+++ b/Figures_Tables/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ecchase/Desktop/Research/Jerel Flint/Flint_Community_Engagement/Figures_Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86A7877-EE13-0F4A-B594-3832B2E6639D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B62F21-AE8F-6545-A628-2DBE3651AB3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{AE4FA38A-5CC6-2F4D-B54C-968C4E2D5875}"/>
+    <workbookView xWindow="12760" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{AE4FA38A-5CC6-2F4D-B54C-968C4E2D5875}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -487,18 +487,6 @@
     <t>   7 (24.1) </t>
   </si>
   <si>
-    <t>1.98 (1.37)</t>
-  </si>
-  <si>
-    <t>1.59 (1.68)</t>
-  </si>
-  <si>
-    <t>1.19 (1.23)</t>
-  </si>
-  <si>
-    <t>1.69 (1.40)</t>
-  </si>
-  <si>
     <t>Total symptoms after April 2014 (mean (SD))</t>
   </si>
   <si>
@@ -1046,6 +1034,18 @@
   </si>
   <si>
     <t>0.7 (0.3,1.8)</t>
+  </si>
+  <si>
+    <t>1.7 (1.4)</t>
+  </si>
+  <si>
+    <t>2.0 (1.4)</t>
+  </si>
+  <si>
+    <t>1.6 (1.7)</t>
+  </si>
+  <si>
+    <t>1.2 (1.2)</t>
   </si>
 </sst>
 </file>
@@ -1479,16 +1479,16 @@
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F3" s="1">
         <v>0.69</v>
@@ -1533,7 +1533,7 @@
         <v>39</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1790,19 +1790,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F19" s="1">
         <v>0.08</v>
@@ -1814,19 +1814,19 @@
         <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1835,16 +1835,16 @@
         <v>31</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F21" s="1">
         <v>0.57999999999999996</v>
@@ -1855,16 +1855,16 @@
         <v>73</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F22" s="1">
         <v>0.57999999999999996</v>
@@ -1881,7 +1881,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1894,7 +1894,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>32</v>
@@ -1944,7 +1944,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -2092,7 +2092,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -2166,7 +2166,7 @@
         <v>3</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2314,7 +2314,7 @@
         <v>3</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -2377,22 +2377,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>153</v>
+        <v>333</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>150</v>
+        <v>334</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>151</v>
+        <v>335</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>152</v>
+        <v>336</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G27" s="1"/>
     </row>
@@ -2448,602 +2448,605 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="21" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -3051,17 +3054,17 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="4" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -3069,17 +3072,17 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -3087,23 +3090,23 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -3111,10 +3114,10 @@
       <c r="H22" s="1"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update to provide sensitivity analyses on missing data.
</commit_message>
<xml_diff>
--- a/Figures_Tables/tables.xlsx
+++ b/Figures_Tables/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ecchase/Desktop/Research/Jerel Flint/Flint_Community_Engagement/Figures_Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B62F21-AE8F-6545-A628-2DBE3651AB3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA606A39-2993-264B-981F-10BA36FCEE89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12760" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{AE4FA38A-5CC6-2F4D-B54C-968C4E2D5875}"/>
+    <workbookView xWindow="6920" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{AE4FA38A-5CC6-2F4D-B54C-968C4E2D5875}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -2448,15 +2448,15 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="21" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>

</xml_diff>